<commit_message>
adds all ecept 3
</commit_message>
<xml_diff>
--- a/articles/2021-05-17-why-should-we-care-about-obesity/raw/Figures.xlsx
+++ b/articles/2021-05-17-why-should-we-care-about-obesity/raw/Figures.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rachelgriffith/Dropbox/ECO/ObesityWeek/MondayObesity/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\OneDrive\Github\eco\ecovisualisations\articles\2021-05-17-why-should-we-care-about-obesity\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DD2647D-2950-1749-A52E-BF2B6A45E6F2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C8CD16D5-E4E2-4088-9A11-EFC29C501225}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30260" yWindow="-460" windowWidth="27240" windowHeight="15560" xr2:uid="{00E1CDBB-1C5F-904A-B188-3F99D9E23A7E}"/>
+    <workbookView xWindow="840" yWindow="-90" windowWidth="18450" windowHeight="10980" xr2:uid="{00E1CDBB-1C5F-904A-B188-3F99D9E23A7E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -42,9 +42,6 @@
     <t>% morbidly obese</t>
   </si>
   <si>
-    <t>Figure 2</t>
-  </si>
-  <si>
     <t>Obese</t>
   </si>
   <si>
@@ -154,13 +151,16 @@
       <t>6</t>
     </r>
   </si>
+  <si>
+    <t>Category</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
@@ -300,7 +300,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="6" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -632,13 +632,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1313F6D-79CC-C440-B23A-AD846F85E87D}">
   <dimension ref="A2:AA60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="B52" sqref="B52"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.8"/>
   <sheetData>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.8">
       <c r="B2" s="1">
         <v>1993</v>
       </c>
@@ -718,7 +718,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.8">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -801,7 +801,7 @@
         <v>27.720880901508465</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.8">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -884,18 +884,21 @@
         <v>3.1579999090682467</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.8">
       <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" t="s">
         <v>2</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>3</v>
       </c>
-      <c r="C7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.8">
+      <c r="A8">
+        <v>1</v>
+      </c>
       <c r="B8">
         <v>27.458031783928998</v>
       </c>
@@ -903,7 +906,10 @@
         <v>7.5251809296426204</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.8">
+      <c r="A9">
+        <v>2</v>
+      </c>
       <c r="B9">
         <v>26.560227367717101</v>
       </c>
@@ -911,7 +917,10 @@
         <v>6.80431329933963</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.8">
+      <c r="A10">
+        <v>3</v>
+      </c>
       <c r="B10">
         <v>25.106422018348599</v>
       </c>
@@ -919,7 +928,10 @@
         <v>5.9963302752293597</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.8">
+      <c r="A11">
+        <v>4</v>
+      </c>
       <c r="B11">
         <v>22.619951178485699</v>
       </c>
@@ -927,7 +939,10 @@
         <v>5.1303616484440697</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.8">
+      <c r="A12">
+        <v>5</v>
+      </c>
       <c r="B12">
         <v>20.961725067385402</v>
       </c>
@@ -935,7 +950,10 @@
         <v>4.3471698113207502</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.8">
+      <c r="A13">
+        <v>6</v>
+      </c>
       <c r="B13">
         <v>19.174965079079001</v>
       </c>
@@ -943,7 +961,10 @@
         <v>3.73541206686793</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.8">
+      <c r="A14">
+        <v>7</v>
+      </c>
       <c r="B14">
         <v>18.262323653406799</v>
       </c>
@@ -951,7 +972,10 @@
         <v>3.4456770060528998</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.8">
+      <c r="A15">
+        <v>8</v>
+      </c>
       <c r="B15">
         <v>16.259479696649699</v>
       </c>
@@ -959,7 +983,10 @@
         <v>2.7071133723720799</v>
       </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.8">
+      <c r="A16">
+        <v>9</v>
+      </c>
       <c r="B16">
         <v>14.9565300468138</v>
       </c>
@@ -967,7 +994,10 @@
         <v>2.4242858507690799</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.8">
+      <c r="A17">
+        <v>10</v>
+      </c>
       <c r="B17">
         <v>11.9477543538039</v>
       </c>
@@ -975,22 +1005,22 @@
         <v>1.58799266727773</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A19" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.8">
       <c r="B20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" t="s">
         <v>19</v>
       </c>
-      <c r="C20" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:3" ht="17.25" x14ac:dyDescent="0.8">
       <c r="A21" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B21" s="8">
         <v>21.4938088162457</v>
@@ -999,9 +1029,9 @@
         <v>12.9888458911905</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" ht="17.25" x14ac:dyDescent="0.8">
       <c r="A22" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B22" s="8">
         <v>22.459263941564799</v>
@@ -1010,9 +1040,9 @@
         <v>13.5534424356201</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" ht="17.25" x14ac:dyDescent="0.8">
       <c r="A23" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B23" s="8">
         <v>22.6367630385488</v>
@@ -1021,9 +1051,9 @@
         <v>13.294991235153899</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A24" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B24" s="8">
         <v>23.461626696313601</v>
@@ -1032,9 +1062,9 @@
         <v>13.641194087527801</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A25" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B25" s="8">
         <v>23.678681696110502</v>
@@ -1043,9 +1073,9 @@
         <v>13.8109389106229</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A26" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B26" s="8">
         <v>24.318098046443101</v>
@@ -1054,9 +1084,9 @@
         <v>13.6845444705707</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A27" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B27" s="8">
         <v>24.189784806844699</v>
@@ -1065,9 +1095,9 @@
         <v>13.0002448257029</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A28" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B28" s="8">
         <v>24.667188723570899</v>
@@ -1076,9 +1106,9 @@
         <v>13.0849283167164</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A29" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B29" s="8">
         <v>24.7545745959663</v>
@@ -1087,9 +1117,9 @@
         <v>12.744581445182099</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A30" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B30" s="8">
         <v>25.664152989304601</v>
@@ -1098,9 +1128,9 @@
         <v>13.260079598546501</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A31" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B31" s="8">
         <v>26.206332140507399</v>
@@ -1109,9 +1139,9 @@
         <v>12.7646177932067</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A32" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B32" s="8">
         <v>26.734121851000001</v>
@@ -1120,9 +1150,9 @@
         <v>13.253711536999999</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A33" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B33" s="8">
         <v>26.9207156639186</v>
@@ -1131,9 +1161,9 @@
         <v>13.037445776983899</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A34" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B34" s="8">
         <v>27.2262153453953</v>
@@ -1142,17 +1172,17 @@
         <v>13.910078252813801</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" ht="16.75" thickBot="1" x14ac:dyDescent="0.95">
       <c r="A35" s="7"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A36" s="6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="17.25" x14ac:dyDescent="0.8">
       <c r="A37" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B37" s="8">
         <v>4.82813273897969</v>
@@ -1161,9 +1191,9 @@
         <v>1.72547234236285</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" ht="17.25" x14ac:dyDescent="0.8">
       <c r="A38" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B38" s="8">
         <v>5.2289647422390804</v>
@@ -1172,9 +1202,9 @@
         <v>1.7773333877484401</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" ht="17.25" x14ac:dyDescent="0.8">
       <c r="A39" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B39" s="8">
         <v>5.3500566893424004</v>
@@ -1183,9 +1213,9 @@
         <v>1.6938803647751699</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A40" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B40" s="8">
         <v>5.5817318721654603</v>
@@ -1194,9 +1224,9 @@
         <v>1.87614723215148</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A41" s="9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B41" s="8">
         <v>5.5118110236220499</v>
@@ -1205,9 +1235,9 @@
         <v>1.9109238639783299</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A42" s="9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B42" s="8">
         <v>5.7611500184297801</v>
@@ -1216,9 +1246,9 @@
         <v>1.8418990034710601</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A43" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B43" s="8">
         <v>5.5427978814030103</v>
@@ -1227,9 +1257,9 @@
         <v>1.75332868792256</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A44" s="9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B44" s="8">
         <v>5.9949534499260402</v>
@@ -1238,9 +1268,9 @@
         <v>1.71748781020304</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A45" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B45" s="8">
         <v>5.9102444236676899</v>
@@ -1249,9 +1279,9 @@
         <v>1.76871465205325</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A46" s="9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B46" s="8">
         <v>6.3811260617411696</v>
@@ -1260,9 +1290,9 @@
         <v>1.87229624502509</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A47" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B47" s="8">
         <v>6.57605468812684</v>
@@ -1271,9 +1301,9 @@
         <v>1.67449458852359</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A48" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B48" s="8">
         <v>7.0365921270999996</v>
@@ -1282,9 +1312,9 @@
         <v>1.9673218877</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A49" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B49" s="8">
         <v>7.1814886277261296</v>
@@ -1293,9 +1323,9 @@
         <v>1.9775452921663701</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A50" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B50" s="8">
         <v>7.3752788301525998</v>
@@ -1304,73 +1334,73 @@
         <v>2.06374549110047</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="77" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:3" ht="75.25" x14ac:dyDescent="0.8">
       <c r="A52" t="s">
+        <v>22</v>
+      </c>
+      <c r="B52" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B52" s="14" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A53" s="11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B53" s="13">
         <v>530.4</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A54" s="11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B54" s="13">
         <v>568.1</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A55" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B55" s="13">
         <v>709.8</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A56" s="11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B56" s="13">
         <v>845.9</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A57" s="12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B57" s="13">
         <v>995.5</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A58" s="12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B58" s="13">
         <v>1158.5999999999999</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A59" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B59" s="13">
         <v>1322.8</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.8">
       <c r="A60" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B60" s="13">
         <v>1615</v>

</xml_diff>